<commit_message>
Actualización casos de prueba
</commit_message>
<xml_diff>
--- a/tests/Casos de prueba API .xlsx
+++ b/tests/Casos de prueba API .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
   <si>
     <t>Pruebas API usuarios</t>
   </si>
@@ -101,20 +101,6 @@
             'password' =&gt; "hola123"</t>
   </si>
   <si>
-    <t>Crear usuario sin contraseña</t>
-  </si>
-  <si>
-    <t>name' =&gt; 'Link Creado', 
-            'lastname' =&gt; 'En Test',
-            'email' =&gt; 'linkuardo@yahoo.com',
-            'document' =&gt; '102010201',
-            'phone' =&gt; '310292929',
-            'password' =&gt; ""</t>
-  </si>
-  <si>
-    <t>El servidor retorna 500. El servidor no crea el usuario.</t>
-  </si>
-  <si>
     <t>Eliminar usuario</t>
   </si>
   <si>
@@ -135,7 +121,7 @@
             'user_id' =&gt; $lastUserId]);</t>
   </si>
   <si>
-    <t>El servidor retorna 500. El servidor crea el paseador correctamente.</t>
+    <t>El servidor retorna 200. El servidor crea el paseador correctamente.</t>
   </si>
   <si>
     <t>Crear paseador con slogan incorrecto</t>
@@ -157,17 +143,371 @@
     <t>Eliminar paseador</t>
   </si>
   <si>
+    <t>Debe retornar 200 y eliminar el usuario de dicho paseador</t>
+  </si>
+  <si>
+    <t>Crear dueño de tienda exitoso</t>
+  </si>
+  <si>
+    <t>user_id' =&gt; $lastUserId</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y crear el dueño de tienda</t>
+  </si>
+  <si>
+    <t>El servidor retorna 500. El servidor crea el usuario correctamente.</t>
+  </si>
+  <si>
+    <t>Eliminar dueño de tienda</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y eliminar el usuario de dicho dueño de tienda</t>
+  </si>
+  <si>
+    <t>Crear dueño de mascota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address' =&gt; 'Calle 10',
+            'user_id' =&gt; $lastUserId
+</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y crear un usuario</t>
+  </si>
+  <si>
+    <t>El servirdor retorna 500 y crea el usuario</t>
+  </si>
+  <si>
+    <t>Crear dueño de mascota con dirección incorrecta</t>
+  </si>
+  <si>
+    <t>address' =&gt; '',
+            'user_id' =&gt; $lastUserId</t>
+  </si>
+  <si>
+    <t>El servidor retorna 422. El servidor no crea un Dueño de mascota</t>
+  </si>
+  <si>
+    <t>Eliminar dueño de mascota</t>
+  </si>
+  <si>
     <t>Debe retornar 200 y crear el usuario de dicho paseador</t>
   </si>
   <si>
-    <t>Crear dueño de tienda 
-exitoso</t>
-  </si>
-  <si>
-    <t>user_id' =&gt; $lastUserId</t>
-  </si>
-  <si>
-    <t>El servidor retorna 500. El servidor crea el usuario correctamente.</t>
+    <t>Crear mascota exitosamente</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Firulais', 
+            'species' =&gt; 'dog',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '12',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y crear a la mascota</t>
+  </si>
+  <si>
+    <t>El servidor retorna 200. El servidor crea a la mascota correctamente</t>
+  </si>
+  <si>
+    <t>Crear mascota con nombre erroneo</t>
+  </si>
+  <si>
+    <t>name' =&gt; '', 
+            'species' =&gt; 'dog',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '12',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Debe retornar 422 y no crear la mascota</t>
+  </si>
+  <si>
+    <t>El servidor retorna 422. El servidor no crea una mascota</t>
+  </si>
+  <si>
+    <t>Crear mascota con especie erronea</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Firulais', 
+            'species' =&gt; '',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '12',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Crear mascota con raza incorrecta</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Firulais', 
+            'species' =&gt; 'dog',
+            'race' =&gt; '',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '12',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Crear mascota con sexo incorrecto</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Firulais', 
+            'species' =&gt; 'dog',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; '',
+            'age' =&gt; '12',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Crear mascota con edad incorrecta</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Firulais', 
+            'species' =&gt; 'dog',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Crear mascota con personalidad incorrecta</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'name' =&gt; 'Firulais', 
+            'species' =&gt; 'dog',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '12',
+            'personality' =&gt; '',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; 'medium'</t>
+  </si>
+  <si>
+    <t>Crear mascota con tamaño incorrecto</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Firulais', 
+            'species' =&gt; 'dog',
+            'race' =&gt; 'Cocker spaniel',
+            'owner_id' =&gt; $lastUserId,
+            'sex' =&gt; 'Macho',
+            'age' =&gt; '12',
+            'personality' =&gt; 'shy',
+            'commentary' =&gt; 'Le gustan las galletas',
+            'size' =&gt; ''</t>
+  </si>
+  <si>
+    <t>Eliminar la mascota</t>
+  </si>
+  <si>
+    <t>deleteJson('api/v1/pets/'.$lastPetId)</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y eliminar la mascota creada</t>
+  </si>
+  <si>
+    <t>El servidor retorna 200 y elimina a la mascota correctamente</t>
+  </si>
+  <si>
+    <t>Crear tienda exitosamente</t>
+  </si>
+  <si>
+    <t>store_name' =&gt; 'La Tienda Prueba', 
+            'slogan' =&gt; 'Vendemos cosas :D',
+            'nit' =&gt; '10203020',
+            'owner_id' =&gt; $lastUserId,
+            'description' =&gt; 'Tienda de juguetes experimentales',
+            'schedule' =&gt; 'Toda la semana de 1 a 9 PM',
+            'address' =&gt; 'Cra 102',
+            'phone_number' =&gt; '8910000'</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y crear la tienda</t>
+  </si>
+  <si>
+    <t>El retorna 200 y crea la tienda exitosamente</t>
+  </si>
+  <si>
+    <t>Crear tienda con nombre</t>
+  </si>
+  <si>
+    <t>store_name' =&gt; '', 
+            'slogan' =&gt; 'Vendemos cosas :D',
+            'nit' =&gt; '10203020',
+            'owner_id' =&gt; $lastUserId,
+            'description' =&gt; 'Tienda de juguetes experimentales',
+            'schedule' =&gt; 'Toda la semana de 1 a 9 PM',
+            'address' =&gt; 'Cra 102',
+            'phone_number' =&gt; '8910000'</t>
+  </si>
+  <si>
+    <t>Debe retornar 422 y no crear la tienda</t>
+  </si>
+  <si>
+    <t>El servidor retorna 422. El servidor no crea una tienda</t>
+  </si>
+  <si>
+    <t>Crear tienda con nit</t>
+  </si>
+  <si>
+    <t>store_name' =&gt; 'La Tienda Prueba', 
+            'slogan' =&gt; 'Vendemos cosas :D',
+            'nit' =&gt; '1020302',
+            'owner_id' =&gt; $lastUserId,
+            'description' =&gt; 'Tienda de juguetes experimentales',
+            'schedule' =&gt; 'Toda la semana de 1 a 9 PM',
+            'address' =&gt; 'Cra 102',
+            'phone_number' =&gt; '8910000'</t>
+  </si>
+  <si>
+    <t>Crear tienda con teléfono</t>
+  </si>
+  <si>
+    <t>store_name' =&gt; 'La Tienda Prueba', 
+            'slogan' =&gt; 'Vendemos cosas :D',
+            'nit' =&gt; '10203020',
+            'owner_id' =&gt; $lastUserId,
+            'description' =&gt; 'Tienda de juguetes experimentales',
+            'schedule' =&gt; 'Toda la semana de 1 a 9 PM',
+            'address' =&gt; 'Cra 102',
+            'phone_number' =&gt; 'pepe'</t>
+  </si>
+  <si>
+    <t>Crear tienda con direccion</t>
+  </si>
+  <si>
+    <t>store_name' =&gt; 'La Tienda Prueba', 
+            'slogan' =&gt; 'Vendemos cosas :D',
+            'nit' =&gt; '10203020',
+            'owner_id' =&gt; $lastUserId,
+            'description' =&gt; 'Tienda de juguetes experimentales',
+            'schedule' =&gt; 'Toda la semana de 1 a 9 PM',
+            'address' =&gt; '',
+            'phone_number' =&gt; '8910000'</t>
+  </si>
+  <si>
+    <t>Eliminar tienda</t>
+  </si>
+  <si>
+    <t>deleteJson('api/v1/stores/'.$lastStoreId);</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y eliminar la tienda</t>
+  </si>
+  <si>
+    <t>El servidor retorna 200 y elimina la tienda</t>
+  </si>
+  <si>
+    <t>Crear un producto exitosamente</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Sopa para gatos', 
+            'price' =&gt; '10000',
+            'discount' =&gt; '10',
+            'quantity' =&gt; '100',
+            'store_id' =&gt; $lastStoreId,
+            'description' =&gt; 'Es una sopa hecha de comida para gatos'</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y crear el producto</t>
+  </si>
+  <si>
+    <t>El servidor retorna 200 y crea el producto</t>
+  </si>
+  <si>
+    <t>Crear un producto sin nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name' =&gt; '', 
+            'price' =&gt; '10000',
+            'discount' =&gt; '10',
+            'quantity' =&gt; '100',
+            'store_id' =&gt; $lastStoreId,
+            'description' =&gt; 'Es una sopa hecha de comida para gatos'
+</t>
+  </si>
+  <si>
+    <t>Debe retornar 422 y no crear el producto</t>
+  </si>
+  <si>
+    <t>El servidor retorna 422 y no crea el producto</t>
+  </si>
+  <si>
+    <t>Crear un producto con precio incorrecto</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Sopa para gatos', 
+            'price' =&gt; 'Muy cara',
+            'discount' =&gt; '10',
+            'quantity' =&gt; '100',
+            'store_id' =&gt; $lastStoreId,
+            'description' =&gt; 'Es una sopa hecha de comida para gatos'</t>
+  </si>
+  <si>
+    <t>Crear un producto con descuento nulo</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Sopa para gatos', 
+            'price' =&gt; '10000',
+            'discount' =&gt; '',
+            'quantity' =&gt; '100',
+            'store_id' =&gt; $lastStoreId,
+            'description' =&gt; 'Es una sopa hecha de comida para gatos'</t>
+  </si>
+  <si>
+    <t>Crear un producto con cantidad incorrecta</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Sopa para gatos', 
+            'price' =&gt; '10000',
+            'discount' =&gt; '10',
+            'quantity' =&gt; 'No hay',
+            'store_id' =&gt; $lastStoreId,
+            'description' =&gt; 'Es una sopa hecha de comida para gatos'</t>
+  </si>
+  <si>
+    <t>Crear un producto con descripción nula</t>
+  </si>
+  <si>
+    <t>name' =&gt; 'Sopa para gatos', 
+            'price' =&gt; '10000',
+            'discount' =&gt; '10',
+            'quantity' =&gt; '100',
+            'store_id' =&gt; $lastStoreId,
+            'description' =&gt; ''</t>
+  </si>
+  <si>
+    <t>Eliminar un producto</t>
+  </si>
+  <si>
+    <t>deleteJson('api/v1/products/'.$lastProductId);</t>
+  </si>
+  <si>
+    <t>Debe retornar 200 y eliminar el producto</t>
+  </si>
+  <si>
+    <t>El servidor retorna 200 y elimina el producto</t>
   </si>
 </sst>
 </file>
@@ -249,7 +589,9 @@
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -468,9 +810,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.43"/>
-    <col customWidth="1" min="2" max="2" width="21.43"/>
-    <col customWidth="1" min="3" max="3" width="42.86"/>
-    <col customWidth="1" min="4" max="4" width="49.71"/>
+    <col customWidth="1" min="2" max="2" width="42.71"/>
+    <col customWidth="1" min="3" max="3" width="56.57"/>
+    <col customWidth="1" min="4" max="4" width="56.0"/>
     <col customWidth="1" min="5" max="5" width="65.71"/>
   </cols>
   <sheetData>
@@ -605,14 +947,14 @@
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
@@ -620,13 +962,13 @@
         <v>8.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>27</v>
@@ -642,11 +984,11 @@
       <c r="C11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -654,15 +996,15 @@
         <v>10.0</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -671,16 +1013,16 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>13</v>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14">
@@ -688,16 +1030,16 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
@@ -705,179 +1047,442 @@
         <v>13.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3">
         <v>14.0</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="B16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="3">
         <v>15.0</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3">
         <v>16.0</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="3">
         <v>17.0</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="B19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3">
         <v>18.0</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3">
         <v>19.0</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="B21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3">
         <v>20.0</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="B22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="3">
         <v>21.0</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3">
         <v>22.0</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="B24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3">
         <v>23.0</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3">
         <v>24.0</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="B26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3">
         <v>25.0</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3">
         <v>26.0</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="B28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="3">
         <v>27.0</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="B29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3">
         <v>28.0</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="B30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3">
         <v>29.0</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="B31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3">
         <v>30.0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="B32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="3">
         <v>31.0</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="B33" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3">
+        <v>32.0</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3">
+        <v>33.0</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3">
+        <v>34.0</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3">
+        <v>36.0</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3">
+        <v>37.0</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3">
+        <v>38.0</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>

</xml_diff>